<commit_message>
✨ Update Product Owner report tasks
</commit_message>
<xml_diff>
--- a/docs/GL/Product Owner report.xlsx
+++ b/docs/GL/Product Owner report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26105"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D8BA568-471A-4D1D-A1DD-803A1136E502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB84229A-A6AC-443B-8AFE-8E979339C81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Development Task</t>
   </si>
@@ -45,7 +45,7 @@
     <t>Dylan</t>
   </si>
   <si>
-    <t>Create a scrum master excel report</t>
+    <t>Non development Task #83</t>
   </si>
   <si>
     <t>Development Task #67</t>
@@ -54,6 +54,9 @@
     <t>Development Task #69</t>
   </si>
   <si>
+    <t>Non development Task #85</t>
+  </si>
+  <si>
     <t>Matis</t>
   </si>
   <si>
@@ -66,7 +69,7 @@
     <t>PA</t>
   </si>
   <si>
-    <t>Create a product owner excel report</t>
+    <t>Non development Task #84</t>
   </si>
   <si>
     <t>Development Task #63</t>
@@ -76,6 +79,9 @@
   </si>
   <si>
     <t>Development Task #65</t>
+  </si>
+  <si>
+    <t>Non development Task #86</t>
   </si>
 </sst>
 </file>
@@ -529,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -583,7 +589,9 @@
     </row>
     <row r="8" spans="1:4">
       <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="10" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="C9" s="1"/>
@@ -591,16 +599,16 @@
     </row>
     <row r="10" spans="1:4" ht="18.75">
       <c r="C10" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="C11" s="1"/>
       <c r="D11" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -617,28 +625,33 @@
     </row>
     <row r="15" spans="1:4" ht="18.75">
       <c r="C15" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="C16" s="1"/>
       <c r="D16" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="3:4">
       <c r="C17" s="1"/>
       <c r="D17" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="3:4">
       <c r="C18" s="3"/>
       <c r="D18" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4">
+      <c r="D19" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
✨ Update Product Owner report
</commit_message>
<xml_diff>
--- a/docs/GL/Product Owner report.xlsx
+++ b/docs/GL/Product Owner report.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26105"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26111"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB84229A-A6AC-443B-8AFE-8E979339C81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F551CC3A-1B46-47BA-99DD-F05832FA0330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Development Task</t>
   </si>
@@ -42,6 +42,9 @@
     <t>For the 16/01/2023</t>
   </si>
   <si>
+    <t>16/01 -&gt; 24/01 | Sprint 1 - UC1</t>
+  </si>
+  <si>
     <t>Dylan</t>
   </si>
   <si>
@@ -51,10 +54,13 @@
     <t>Development Task #67</t>
   </si>
   <si>
+    <t>Non development Task #85</t>
+  </si>
+  <si>
     <t>Development Task #69</t>
   </si>
   <si>
-    <t>Non development Task #85</t>
+    <t>Development Task #71</t>
   </si>
   <si>
     <t>Matis</t>
@@ -66,29 +72,41 @@
     <t>Development Task #68</t>
   </si>
   <si>
+    <t>Development Task #72</t>
+  </si>
+  <si>
     <t>PA</t>
   </si>
   <si>
     <t>Non development Task #84</t>
   </si>
   <si>
+    <t>Development Task #65</t>
+  </si>
+  <si>
+    <t>Non development Task #86</t>
+  </si>
+  <si>
+    <t>Development Task #70</t>
+  </si>
+  <si>
     <t>Development Task #63</t>
   </si>
   <si>
+    <t>Development Task #75</t>
+  </si>
+  <si>
     <t>Development Task #64</t>
   </si>
   <si>
-    <t>Development Task #65</t>
-  </si>
-  <si>
-    <t>Non development Task #86</t>
+    <t>Non development Task #87</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +128,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -209,18 +233,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,124 +566,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="34.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75">
-      <c r="C4" s="5" t="s">
+    <row r="4" spans="1:5" ht="18.75">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="18.75">
-      <c r="C5" s="6" t="s">
+      <c r="E4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="10" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="18.75">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="C6" s="1"/>
-      <c r="D6" s="9" t="s">
+      <c r="D5" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E5" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" s="16"/>
+      <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="C7" s="1"/>
-      <c r="D7" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" s="2"/>
+      <c r="E7" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="C8" s="1"/>
-      <c r="D8" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="C9" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="C9" s="3"/>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" ht="18.75">
-      <c r="C10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="C11" s="1"/>
-      <c r="D11" s="9" t="s">
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" ht="18.75">
+      <c r="C10" s="17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D10" s="10"/>
+      <c r="E10" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="C11" s="16"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="C14" s="1"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="C14" s="3"/>
       <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" ht="18.75">
-      <c r="C15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="C16" s="1"/>
-      <c r="D16" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4">
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:5" ht="18.75">
+      <c r="C15" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="C16" s="16"/>
+      <c r="D16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5">
       <c r="C17" s="1"/>
-      <c r="D17" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4">
+      <c r="D17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
       <c r="C18" s="3"/>
-      <c r="D18" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4">
-      <c r="D19" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="D18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5">
+      <c r="C19" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
✨ Add testing procedure document
</commit_message>
<xml_diff>
--- a/docs/GL/Product Owner report.xlsx
+++ b/docs/GL/Product Owner report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26111"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F551CC3A-1B46-47BA-99DD-F05832FA0330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2737FE9F-2F30-4C0A-9254-A798E055DEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Development Task</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Development Task #69</t>
   </si>
   <si>
-    <t>Development Task #71</t>
+    <t>Non development Task #88</t>
   </si>
   <si>
     <t>Matis</t>
@@ -72,7 +72,7 @@
     <t>Development Task #68</t>
   </si>
   <si>
-    <t>Development Task #72</t>
+    <t>Non development Task #93</t>
   </si>
   <si>
     <t>PA</t>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Non development Task #87</t>
+  </si>
+  <si>
+    <t>Development Task #89</t>
+  </si>
+  <si>
+    <t>Non development Task #94</t>
   </si>
 </sst>
 </file>
@@ -136,7 +142,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,8 +161,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -229,11 +241,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -249,9 +272,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -614,7 +639,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="C6" s="16"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
@@ -625,14 +650,13 @@
     <row r="7" spans="1:5">
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5">
       <c r="C9" s="3"/>
@@ -640,7 +664,7 @@
       <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5" ht="18.75">
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="10"/>
@@ -649,7 +673,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="C11" s="16"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="2"/>
       <c r="E11" s="12" t="s">
         <v>13</v>
@@ -658,7 +682,7 @@
     <row r="12" spans="1:5">
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="11" t="s">
         <v>14</v>
       </c>
     </row>
@@ -673,7 +697,7 @@
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" ht="18.75">
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="11" t="s">
@@ -684,7 +708,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="C16" s="16"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="8" t="s">
         <v>18</v>
       </c>
@@ -702,16 +726,27 @@
       </c>
     </row>
     <row r="18" spans="3:5">
-      <c r="C18" s="3"/>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="19" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="3:5">
-      <c r="C19" s="15"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5">
+      <c r="C20" s="3"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="11" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
📝 Update PO report with new sprint + Testing procedure for UC2
</commit_message>
<xml_diff>
--- a/docs/GL/Product Owner report.xlsx
+++ b/docs/GL/Product Owner report.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26111"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\Documents\GitHub\gp-dam-teamflexsante\docs\GL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAF5DB6-C865-436A-9D3F-8045CE3CFA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F980E94-B2FB-44FB-82BB-12073D260D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Development Task</t>
   </si>
@@ -50,6 +45,9 @@
     <t>16/01 -&gt; 24/01 | Sprint 1 - UC1</t>
   </si>
   <si>
+    <t>24/01 -&gt; 31/01 | Sprint 2 - UC2</t>
+  </si>
+  <si>
     <t>Dylan</t>
   </si>
   <si>
@@ -59,24 +57,42 @@
     <t>Development Task #67</t>
   </si>
   <si>
+    <t>Development Task #74</t>
+  </si>
+  <si>
     <t>Non development Task #85</t>
   </si>
   <si>
     <t>Development Task #69</t>
   </si>
   <si>
+    <t>Development Task #77</t>
+  </si>
+  <si>
     <t>Non development Task #88</t>
   </si>
   <si>
+    <t>Development Task #99</t>
+  </si>
+  <si>
+    <t>Development Task #100</t>
+  </si>
+  <si>
     <t>Matis</t>
   </si>
   <si>
     <t>Development Task #66</t>
   </si>
   <si>
+    <t>Development Task #73</t>
+  </si>
+  <si>
     <t>Development Task #68</t>
   </si>
   <si>
+    <t>Development Task #76</t>
+  </si>
+  <si>
     <t>Non development Task #93</t>
   </si>
   <si>
@@ -89,18 +105,21 @@
     <t>Development Task #65</t>
   </si>
   <si>
+    <t>Development Task #78</t>
+  </si>
+  <si>
     <t>Non development Task #86</t>
   </si>
   <si>
     <t>Development Task #70</t>
   </si>
   <si>
+    <t>Development Task #75</t>
+  </si>
+  <si>
     <t>Development Task #63</t>
   </si>
   <si>
-    <t>Development Task #75</t>
-  </si>
-  <si>
     <t>Development Task #64</t>
   </si>
   <si>
@@ -111,31 +130,13 @@
   </si>
   <si>
     <t>Non development Task #94</t>
-  </si>
-  <si>
-    <t>24/01 -&gt; 31/01 | Sprint 2 - UC2</t>
-  </si>
-  <si>
-    <t>Development Task #74</t>
-  </si>
-  <si>
-    <t>Development Task #77</t>
-  </si>
-  <si>
-    <t>Development Task #73</t>
-  </si>
-  <si>
-    <t>Development Task #76</t>
-  </si>
-  <si>
-    <t>Development Task #78</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,15 +145,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="14"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,8 +164,6 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -176,25 +176,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFED7D31"/>
-        <bgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -286,30 +286,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -328,7 +326,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -627,243 +625,201 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="40.44140625" customWidth="1"/>
-    <col min="6" max="6" width="40.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" customWidth="1"/>
+    <col min="6" max="6" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4" t="s">
+    </row>
+    <row r="4" spans="1:6" ht="18.75">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75">
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="C6" s="15"/>
+      <c r="D6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="F8" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="C9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75">
+      <c r="C10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="C11" s="15"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="C14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="20"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75">
+      <c r="C15" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="C16" s="15"/>
+      <c r="D16" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="E16" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="F16" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="8" t="s">
+    <row r="17" spans="3:6">
+      <c r="C17" s="1"/>
+      <c r="D17" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="E17" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18" s="1"/>
+      <c r="D18" s="18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="18" t="s">
+      <c r="E18" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="14"/>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20" s="3"/>
+      <c r="E20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
📝 #105 Improve PO report according to Product backlog
</commit_message>
<xml_diff>
--- a/docs/GL/Product Owner report.xlsx
+++ b/docs/GL/Product Owner report.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26202"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F980E94-B2FB-44FB-82BB-12073D260D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3614047-4FC5-4C21-A249-6AE21C6C887C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,9 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
-  <si>
-    <t>Development Task</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+  <si>
+    <t>Type of task</t>
+  </si>
+  <si>
+    <t>All task are clickable and are linked to the Github task board</t>
   </si>
   <si>
     <t>Non Development Task</t>
@@ -42,10 +45,50 @@
     <t>For the 16/01/2023</t>
   </si>
   <si>
-    <t>16/01 -&gt; 24/01 | Sprint 1 - UC1</t>
-  </si>
-  <si>
-    <t>24/01 -&gt; 31/01 | Sprint 2 - UC2</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">16/01 -&gt; 24/01 | </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Sprint 1 - UC1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">24/01 -&gt; 07/02 | </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Sprint 2 - UC2</t>
+    </r>
+  </si>
+  <si>
+    <t>07/02 -&gt; 14/02 | Sprint 3</t>
+  </si>
+  <si>
+    <t>CI / CD</t>
   </si>
   <si>
     <t>Dylan</t>
@@ -60,6 +103,9 @@
     <t>Development Task #74</t>
   </si>
   <si>
+    <t>Non development Task #104</t>
+  </si>
+  <si>
     <t>Non development Task #85</t>
   </si>
   <si>
@@ -69,15 +115,24 @@
     <t>Development Task #77</t>
   </si>
   <si>
+    <t>Backend</t>
+  </si>
+  <si>
     <t>Non development Task #88</t>
   </si>
   <si>
     <t>Development Task #99</t>
   </si>
   <si>
+    <t>Testing</t>
+  </si>
+  <si>
     <t>Development Task #100</t>
   </si>
   <si>
+    <t>Frontend</t>
+  </si>
+  <si>
     <t>Matis</t>
   </si>
   <si>
@@ -87,15 +142,27 @@
     <t>Development Task #73</t>
   </si>
   <si>
+    <t>Integration</t>
+  </si>
+  <si>
     <t>Development Task #68</t>
   </si>
   <si>
     <t>Development Task #76</t>
   </si>
   <si>
+    <t>Dynamization</t>
+  </si>
+  <si>
     <t>Non development Task #93</t>
   </si>
   <si>
+    <t>Use case</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>PA</t>
   </si>
   <si>
@@ -108,35 +175,82 @@
     <t>Development Task #78</t>
   </si>
   <si>
+    <t>Non development Task #105</t>
+  </si>
+  <si>
+    <t>UC 1</t>
+  </si>
+  <si>
+    <t>UC Register / Login / Logout</t>
+  </si>
+  <si>
     <t>Non development Task #86</t>
   </si>
   <si>
-    <t>Development Task #70</t>
-  </si>
-  <si>
     <t>Development Task #75</t>
   </si>
   <si>
+    <t>UC 2</t>
+  </si>
+  <si>
+    <t>UC Health Data</t>
+  </si>
+  <si>
     <t>Development Task #63</t>
   </si>
   <si>
+    <t>Non development Task #87</t>
+  </si>
+  <si>
     <t>Development Task #64</t>
   </si>
   <si>
-    <t>Non development Task #87</t>
-  </si>
-  <si>
     <t>Development Task #89</t>
   </si>
   <si>
     <t>Non development Task #94</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Initialization &amp; Non dev tasks</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>UC1 - Handle Auth</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> &amp; Non dev tasks</t>
+    </r>
+  </si>
+  <si>
+    <t>UC2 - Handle Health data</t>
+  </si>
+  <si>
+    <t>Non dev tasks</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,8 +279,131 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,18 +424,66 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF70AD47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -282,34 +567,189 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -622,206 +1062,344 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="36" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
     <col min="5" max="5" width="40.42578125" customWidth="1"/>
     <col min="6" max="6" width="41.28515625" customWidth="1"/>
+    <col min="7" max="7" width="37.28515625" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" ht="18.75">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="6" t="s">
+      <c r="C1" s="52" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18.75">
-      <c r="C4" s="9" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="18.75">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="18.75">
-      <c r="C5" s="4" t="s">
+      <c r="G4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="H4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="12" t="s">
+    </row>
+    <row r="5" spans="1:8" ht="18.75">
+      <c r="A5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="C6" s="15"/>
-      <c r="D6" s="8" t="s">
+      <c r="E5" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="G5" s="50" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="17" t="s">
+      <c r="H5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="12" t="s">
+    </row>
+    <row r="6" spans="1:8">
+      <c r="D6" s="8"/>
+      <c r="E6" s="31" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="F8" s="12" t="s">
+      <c r="F6" s="29" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="C9" s="3"/>
+      <c r="G6" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="32"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="21"/>
+      <c r="B8" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="32"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="D9" s="2"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="20"/>
-    </row>
-    <row r="10" spans="1:6" ht="18.75">
-      <c r="C10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="C11" s="15"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="12" t="s">
+      <c r="E9" s="33"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="32"/>
+    </row>
+    <row r="10" spans="1:8" ht="18.75">
+      <c r="A10" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="D10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="37"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="19"/>
+      <c r="B11" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="32"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="21"/>
+      <c r="B12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="11" t="s">
+      <c r="H12" s="32"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="D13" s="1"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="C14" s="3"/>
+      <c r="H13" s="32"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="D14" s="2"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="20"/>
-    </row>
-    <row r="15" spans="1:6" ht="18.75">
-      <c r="C15" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="C16" s="15"/>
-      <c r="D16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6">
-      <c r="C17" s="1"/>
-      <c r="D17" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6">
-      <c r="C18" s="1"/>
-      <c r="D18" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="19" t="s">
+      <c r="E14" s="33"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="32"/>
+    </row>
+    <row r="15" spans="1:8" ht="18.75">
+      <c r="A15" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6">
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="12" t="s">
+      <c r="B15" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="20"/>
-    </row>
-    <row r="20" spans="3:6">
-      <c r="C20" s="3"/>
-      <c r="E20" s="11" t="s">
+      <c r="D15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="20"/>
+      <c r="E15" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="32"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="32"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="55"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="32"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="56"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="36"/>
+      <c r="H19" s="32"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="57"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="32"/>
+    </row>
+    <row r="23" spans="1:8" ht="18.75">
+      <c r="D23" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="D24" s="2"/>
+      <c r="E24" s="15">
+        <v>1</v>
+      </c>
+      <c r="F24" s="14">
+        <v>1</v>
+      </c>
+      <c r="G24" s="14">
+        <v>1</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E17" r:id="rId1" xr:uid="{981715B9-BC2C-4009-8CB0-33DD6E28E9EE}"/>
+    <hyperlink ref="E18" r:id="rId2" xr:uid="{7223F42F-06F6-427C-98B7-497B49B4D691}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{D97BB322-117B-4798-81FC-6F7A713AF423}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{E142D021-AFE4-4CCD-849A-9E206B4BCF51}"/>
+    <hyperlink ref="E15" r:id="rId5" xr:uid="{27F01E42-DEEF-44B1-A43A-F00F65BD507D}"/>
+    <hyperlink ref="E16" r:id="rId6" xr:uid="{1C222B23-861A-484A-9F46-FCD3AC36A7CB}"/>
+    <hyperlink ref="F5" r:id="rId7" xr:uid="{31A8B9A7-138C-454B-AF7D-5AAC482F7C93}"/>
+    <hyperlink ref="F6" r:id="rId8" xr:uid="{C0C670FE-DCBE-4CAC-B8C6-2324A21F5F58}"/>
+    <hyperlink ref="F7" r:id="rId9" xr:uid="{C90B4949-741E-49FB-B3D3-F229E0BE7538}"/>
+    <hyperlink ref="F10" r:id="rId10" xr:uid="{2D8914E7-AC02-4ABF-9037-C932DCB448CC}"/>
+    <hyperlink ref="F11" r:id="rId11" xr:uid="{57AE303A-0B69-45DE-AC10-37BA02AF8850}"/>
+    <hyperlink ref="F12" r:id="rId12" xr:uid="{333AC8DA-2AE0-4B4D-A8DA-BD597BC91B3A}"/>
+    <hyperlink ref="F15" r:id="rId13" xr:uid="{FCB534B3-590E-4103-ACB5-65CB59832F92}"/>
+    <hyperlink ref="F16" r:id="rId14" xr:uid="{B6D97C9E-0D43-4261-B538-827E908D9358}"/>
+    <hyperlink ref="F17" r:id="rId15" xr:uid="{C0445A4E-4F30-48BF-9869-02C2887AB511}"/>
+    <hyperlink ref="F18" r:id="rId16" xr:uid="{B4D89713-BCB8-42B3-9F30-C9A64E969C4B}"/>
+    <hyperlink ref="F19" r:id="rId17" xr:uid="{3E29B334-1EE3-4282-8967-C5184BAD7272}"/>
+    <hyperlink ref="G5" r:id="rId18" xr:uid="{0487314B-CC8F-4112-959F-1212E712A365}"/>
+    <hyperlink ref="G6" r:id="rId19" xr:uid="{7DDB687D-9D6D-40FB-A101-D08CBEAB1B5A}"/>
+    <hyperlink ref="G7" r:id="rId20" xr:uid="{A00426EE-4B2E-403F-B9B2-4F0F76DEA697}"/>
+    <hyperlink ref="G8" r:id="rId21" xr:uid="{9780C24C-A65A-4FE6-BC7C-F6BC0B9060AA}"/>
+    <hyperlink ref="G10" r:id="rId22" xr:uid="{6B53C06A-1FCC-4BFF-A569-61AFC87E8A32}"/>
+    <hyperlink ref="G11" r:id="rId23" xr:uid="{41218433-5727-4D83-BE77-9BFD8EE0A16A}"/>
+    <hyperlink ref="G12" r:id="rId24" xr:uid="{27B6CB1C-38CA-4FA4-831D-A66C4768497C}"/>
+    <hyperlink ref="G13" r:id="rId25" xr:uid="{EA8971BF-BE33-4416-9CF7-1ADC22C5AFE0}"/>
+    <hyperlink ref="G18" r:id="rId26" xr:uid="{0D30F1C3-AF43-486A-A061-6033A4C0B1CD}"/>
+    <hyperlink ref="G15" r:id="rId27" xr:uid="{35C16AD4-0D10-4876-BB97-F07DE9A9A81D}"/>
+    <hyperlink ref="G16" r:id="rId28" xr:uid="{DC5223DF-6805-4FDD-B54B-94B7760CDA71}"/>
+    <hyperlink ref="G17" r:id="rId29" xr:uid="{39586FCE-22AD-4D40-A565-21A58327F4D4}"/>
+    <hyperlink ref="H5" r:id="rId30" xr:uid="{E1A44888-C26E-449A-B82A-17A0E4CFD8E3}"/>
+    <hyperlink ref="H15" r:id="rId31" xr:uid="{D9FB72E7-93CB-428C-817B-6ADFFD7874BB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>